<commit_message>
importation des données depuis le fichier. affichage des nouveaux et ajouts dans le base de donnée..
</commit_message>
<xml_diff>
--- a/public/docs/2019-12-03--data.xlsx
+++ b/public/docs/2019-12-03--data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="366">
   <si>
     <t xml:space="preserve">Num structure</t>
   </si>
@@ -1097,6 +1097,27 @@
   </si>
   <si>
     <t xml:space="preserve">dominique21000@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 rue de provence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schiltigheim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STURM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eric.sturm@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 rue de la glacière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strasbourg</t>
   </si>
 </sst>
 </file>
@@ -1209,13 +1230,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E94" activeCellId="0" sqref="E94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E95" activeCellId="0" sqref="E95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -4984,10 +5005,49 @@
       <c r="H89" s="0" t="s">
         <v>358</v>
       </c>
+      <c r="I89" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="J89" s="0" t="n">
+        <v>67300</v>
+      </c>
+      <c r="K89" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="L89" s="0" t="n">
+        <v>685400936</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" s="3" t="n">
+        <v>30784</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <v>67000</v>
+      </c>
+      <c r="K90" s="0" t="s">
+        <v>365</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H89" r:id="rId1" display="dominique21000@gmail.com"/>
+    <hyperlink ref="H90" r:id="rId2" display="eric.sturm@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>